<commit_message>
updated number of words used as input from 4 to 8
</commit_message>
<xml_diff>
--- a/CLIP Model Results.xlsx
+++ b/CLIP Model Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Portable\Documents\GitHub\CMPUT624_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CEB0B5-1810-4D3D-B8F4-E5D8121A3B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30094F1B-17C9-4FE7-B4AB-67415D93E41B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="34">
   <si>
     <t>Text Input</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Test Text Accuracy*</t>
   </si>
   <si>
-    <t>* Accuracies are taken as average over all batches, train accuracy is from last epoch</t>
-  </si>
-  <si>
     <t>Subject ID(s)</t>
   </si>
   <si>
@@ -108,7 +105,28 @@
     <t>8 words</t>
   </si>
   <si>
-    <t>LR=1e-4, batch_size=128, weight_decay=0.2</t>
+    <t>LR=1e-4, batch_size=96, weight_decay=0.2</t>
+  </si>
+  <si>
+    <t>LR=1e-4, batch_size=32, weight_decay=0.2</t>
+  </si>
+  <si>
+    <t>embed_dim=512, image_resolution, layers=(2,2,2,2), width=64, context_length=32, vocab_size, transformer_width, transformer_heads, transformer_layers</t>
+  </si>
+  <si>
+    <t>* Accuracies are taken as average over all batches, train accuracy is from last epoch, batch_size=64 for all evaluations</t>
+  </si>
+  <si>
+    <t>16 words</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Using pre-trained weights for text encoder</t>
+  </si>
+  <si>
+    <t>Leaving out very few samples for testing (16?) and training on all other. Similar to leave-one-out. This might solve the issue of there being too few samples for training.</t>
   </si>
 </sst>
 </file>
@@ -152,10 +170,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,12 +475,12 @@
     <col min="12" max="12" width="23.28515625" customWidth="1"/>
     <col min="13" max="13" width="21.7109375" customWidth="1"/>
     <col min="14" max="14" width="26.5703125" customWidth="1"/>
-    <col min="15" max="15" width="22.140625" customWidth="1"/>
+    <col min="15" max="16" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -484,10 +501,10 @@
         <v>11</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>4</v>
@@ -508,10 +525,13 @@
         <v>17</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -519,7 +539,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -534,7 +554,7 @@
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I2" t="s">
         <v>10</v>
@@ -558,7 +578,7 @@
         <v>3.90625E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -566,7 +586,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -581,7 +601,7 @@
         <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I3" t="s">
         <v>10</v>
@@ -592,20 +612,20 @@
       <c r="K3" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3">
         <v>0.912109375</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3">
         <v>0.9189453125</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3">
         <v>3.90625E-2</v>
       </c>
       <c r="O3">
         <v>2.34375E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -613,22 +633,22 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
         <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" t="s">
-        <v>23</v>
       </c>
       <c r="I4" t="s">
         <v>10</v>
@@ -651,8 +671,9 @@
       <c r="O4" s="1">
         <v>5.078125E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -660,22 +681,22 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
         <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" t="s">
-        <v>23</v>
       </c>
       <c r="I5" t="s">
         <v>10</v>
@@ -686,20 +707,21 @@
       <c r="K5" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="1">
+      <c r="L5">
         <v>0.986328125</v>
       </c>
       <c r="M5" s="1">
         <v>0.984375</v>
       </c>
-      <c r="N5" s="1">
+      <c r="N5">
         <v>5.078125E-2</v>
       </c>
       <c r="O5" s="1">
         <v>5.078125E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P5" s="1"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -707,7 +729,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -722,7 +744,7 @@
         <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I6" t="s">
         <v>10</v>
@@ -733,8 +755,20 @@
       <c r="K6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <v>0.791015625</v>
+      </c>
+      <c r="M6">
+        <v>0.7626953125</v>
+      </c>
+      <c r="N6" s="1">
+        <v>5.859375E-2</v>
+      </c>
+      <c r="O6">
+        <v>3.90625E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -742,7 +776,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
@@ -757,7 +791,7 @@
         <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I7" t="s">
         <v>10</v>
@@ -781,7 +815,7 @@
         <v>2.34375E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -789,54 +823,241 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" t="s">
-        <v>12</v>
-      </c>
       <c r="I8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8">
+        <v>100</v>
+      </c>
+      <c r="K8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0.9873046875</v>
+      </c>
+      <c r="M8">
+        <v>0.9794921875</v>
+      </c>
+      <c r="N8">
+        <v>3.90625E-2</v>
+      </c>
+      <c r="O8">
+        <v>2.734375E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" t="s">
         <v>27</v>
       </c>
-      <c r="K8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>0</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="J9">
+        <v>100</v>
+      </c>
+      <c r="K9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9">
+        <v>0.599609375</v>
+      </c>
+      <c r="M9">
+        <v>0.5712890625</v>
+      </c>
+      <c r="N9">
+        <v>2.734375E-2</v>
+      </c>
+      <c r="O9">
+        <v>3.515625E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" t="s">
         <v>10</v>
       </c>
-      <c r="K9" t="s">
-        <v>13</v>
+      <c r="J10">
+        <v>50</v>
+      </c>
+      <c r="K10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11">
+        <v>50</v>
+      </c>
+      <c r="K11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12">
+        <v>50</v>
+      </c>
+      <c r="K12" t="s">
+        <v>13</v>
+      </c>
+      <c r="P12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13">
+        <v>100</v>
+      </c>
+      <c r="K13" t="s">
+        <v>13</v>
+      </c>
+      <c r="P13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P14" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tried training using multiple subjects, too slow currently
</commit_message>
<xml_diff>
--- a/CLIP Model Results.xlsx
+++ b/CLIP Model Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Portable\Documents\GitHub\CMPUT624_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30094F1B-17C9-4FE7-B4AB-67415D93E41B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2714E046-EB82-4513-9678-22F1473D830D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="41">
   <si>
     <t>Text Input</t>
   </si>
@@ -111,9 +111,6 @@
     <t>LR=1e-4, batch_size=32, weight_decay=0.2</t>
   </si>
   <si>
-    <t>embed_dim=512, image_resolution, layers=(2,2,2,2), width=64, context_length=32, vocab_size, transformer_width, transformer_heads, transformer_layers</t>
-  </si>
-  <si>
     <t>* Accuracies are taken as average over all batches, train accuracy is from last epoch, batch_size=64 for all evaluations</t>
   </si>
   <si>
@@ -126,7 +123,31 @@
     <t>Using pre-trained weights for text encoder</t>
   </si>
   <si>
-    <t>Leaving out very few samples for testing (16?) and training on all other. Similar to leave-one-out. This might solve the issue of there being too few samples for training.</t>
+    <t>embed_dim=512, image_resolution, layers=(2,2,2,2), width=64, context_length=24, vocab_size, transformer_width, transformer_heads, transformer_layers</t>
+  </si>
+  <si>
+    <t>embed_dim=512, image_resolution, layers=(2,2,2,2), width=64, context_length=48, vocab_size, transformer_width, transformer_heads, transformer_layers</t>
+  </si>
+  <si>
+    <t>95/0/5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0 (training), 1 (testing)</t>
+  </si>
+  <si>
+    <t>100/0/100</t>
+  </si>
+  <si>
+    <t>3D fMRI image 8 seconds after first word</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0-2 (training), 3 (testing)</t>
+  </si>
+  <si>
+    <t>300/0/100</t>
+  </si>
+  <si>
+    <t>Data is not shuffled before train/test split. Using pre-trained weights for text encoder</t>
   </si>
 </sst>
 </file>
@@ -170,9 +191,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,15 +475,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
     <col min="3" max="3" width="29.7109375" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" customWidth="1"/>
@@ -525,10 +547,10 @@
         <v>17</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -668,7 +690,7 @@
       <c r="N4">
         <v>3.515625E-2</v>
       </c>
-      <c r="O4" s="1">
+      <c r="O4">
         <v>5.078125E-2</v>
       </c>
       <c r="P4" s="1"/>
@@ -716,7 +738,7 @@
       <c r="N5">
         <v>5.078125E-2</v>
       </c>
-      <c r="O5" s="1">
+      <c r="O5">
         <v>5.078125E-2</v>
       </c>
       <c r="P5" s="1"/>
@@ -761,7 +783,7 @@
       <c r="M6">
         <v>0.7626953125</v>
       </c>
-      <c r="N6" s="1">
+      <c r="N6">
         <v>5.859375E-2</v>
       </c>
       <c r="O6">
@@ -932,7 +954,7 @@
         <v>12</v>
       </c>
       <c r="H10" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="I10" t="s">
         <v>10</v>
@@ -943,13 +965,25 @@
       <c r="K10" t="s">
         <v>13</v>
       </c>
+      <c r="L10">
+        <v>0.88645833333333302</v>
+      </c>
+      <c r="M10">
+        <v>0.89791666666666603</v>
+      </c>
+      <c r="N10">
+        <v>0.1875</v>
+      </c>
+      <c r="O10">
+        <v>0.203125</v>
+      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
         <v>21</v>
@@ -967,7 +1001,7 @@
         <v>12</v>
       </c>
       <c r="H11" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="I11" t="s">
         <v>10</v>
@@ -976,7 +1010,22 @@
         <v>50</v>
       </c>
       <c r="K11" t="s">
-        <v>13</v>
+        <v>34</v>
+      </c>
+      <c r="L11">
+        <v>0.84548611111111105</v>
+      </c>
+      <c r="M11">
+        <v>0.8828125</v>
+      </c>
+      <c r="N11" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="O11" s="2">
+        <v>0.296875</v>
+      </c>
+      <c r="P11" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -984,10 +1033,10 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="D12" t="s">
         <v>8</v>
@@ -1002,7 +1051,7 @@
         <v>12</v>
       </c>
       <c r="H12" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="I12" t="s">
         <v>10</v>
@@ -1011,18 +1060,30 @@
         <v>50</v>
       </c>
       <c r="K12" t="s">
-        <v>13</v>
+        <v>34</v>
+      </c>
+      <c r="L12">
+        <v>0.90625</v>
+      </c>
+      <c r="M12">
+        <v>0.89687499999999998</v>
+      </c>
+      <c r="N12" s="1">
+        <v>0.44791666666666602</v>
+      </c>
+      <c r="O12" s="1">
+        <v>0.4375</v>
       </c>
       <c r="P12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>0</v>
+      <c r="A13" t="s">
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
         <v>21</v>
@@ -1040,24 +1101,119 @@
         <v>12</v>
       </c>
       <c r="H13" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="I13" t="s">
         <v>10</v>
       </c>
       <c r="J13">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="K13" t="s">
-        <v>13</v>
+        <v>36</v>
+      </c>
+      <c r="L13">
+        <v>0.86595394736842102</v>
+      </c>
+      <c r="M13">
+        <v>0.86019736842105199</v>
+      </c>
+      <c r="N13">
+        <v>3.2894736842105199E-2</v>
+      </c>
+      <c r="O13">
+        <v>3.94736842105263E-2</v>
       </c>
       <c r="P13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14">
+        <v>50</v>
+      </c>
+      <c r="K14" t="s">
+        <v>39</v>
+      </c>
       <c r="P14" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" t="s">
+        <v>10</v>
+      </c>
+      <c r="J15">
+        <v>50</v>
+      </c>
+      <c r="K15" t="s">
+        <v>34</v>
+      </c>
+      <c r="L15">
+        <v>0.90798611111111105</v>
+      </c>
+      <c r="M15">
+        <v>0.90885416666666596</v>
+      </c>
+      <c r="N15" s="2">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="O15" s="2">
+        <v>0</v>
+      </c>
+      <c r="P15" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wrote file for compute canada
</commit_message>
<xml_diff>
--- a/CLIP Model Results.xlsx
+++ b/CLIP Model Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Portable\Documents\GitHub\CMPUT624_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2714E046-EB82-4513-9678-22F1473D830D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09977C0C-F200-4AF5-A708-125BA87F3AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="41">
   <si>
     <t>Text Input</t>
   </si>
@@ -90,9 +90,6 @@
     <t>CLIP Hyperparameters</t>
   </si>
   <si>
-    <t>3D fMRI image 6 seconds after first word</t>
-  </si>
-  <si>
     <t>embed_dim=512, image_resolution, layers=(2,2,2,2), width=64, context_length=16, vocab_size, transformer_width, transformer_heads, transformer_layers</t>
   </si>
   <si>
@@ -138,16 +135,19 @@
     <t>100/0/100</t>
   </si>
   <si>
-    <t>3D fMRI image 8 seconds after first word</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0-2 (training), 3 (testing)</t>
   </si>
   <si>
     <t>300/0/100</t>
   </si>
   <si>
-    <t>Data is not shuffled before train/test split. Using pre-trained weights for text encoder</t>
+    <t xml:space="preserve">Data is not shuffled before train/test split. </t>
+  </si>
+  <si>
+    <t>3D fMRI image 6 seconds after 4th words</t>
+  </si>
+  <si>
+    <t>3D fMRI image 8 seconds after 4th words</t>
   </si>
 </sst>
 </file>
@@ -191,10 +191,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q15"/>
+  <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,10 +546,10 @@
         <v>17</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -561,7 +560,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -576,7 +575,7 @@
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I2" t="s">
         <v>10</v>
@@ -608,7 +607,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -623,7 +622,7 @@
         <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I3" t="s">
         <v>10</v>
@@ -655,22 +654,22 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
         <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
       </c>
       <c r="I4" t="s">
         <v>10</v>
@@ -703,22 +702,22 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
         <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" t="s">
-        <v>22</v>
       </c>
       <c r="I5" t="s">
         <v>10</v>
@@ -751,7 +750,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -766,7 +765,7 @@
         <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I6" t="s">
         <v>10</v>
@@ -798,7 +797,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
@@ -813,7 +812,7 @@
         <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I7" t="s">
         <v>10</v>
@@ -845,25 +844,25 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" t="s">
         <v>21</v>
       </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" t="s">
-        <v>22</v>
-      </c>
       <c r="I8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J8">
         <v>100</v>
@@ -892,25 +891,25 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" t="s">
         <v>21</v>
       </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" t="s">
-        <v>22</v>
-      </c>
       <c r="I9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J9">
         <v>100</v>
@@ -936,10 +935,10 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
@@ -954,7 +953,7 @@
         <v>12</v>
       </c>
       <c r="H10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I10" t="s">
         <v>10</v>
@@ -983,10 +982,10 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s">
         <v>8</v>
@@ -1001,7 +1000,7 @@
         <v>12</v>
       </c>
       <c r="H11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I11" t="s">
         <v>10</v>
@@ -1010,22 +1009,22 @@
         <v>50</v>
       </c>
       <c r="K11" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="L11">
-        <v>0.84548611111111105</v>
+        <v>0.70104166666666601</v>
       </c>
       <c r="M11">
-        <v>0.8828125</v>
-      </c>
-      <c r="N11" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="O11" s="2">
-        <v>0.296875</v>
+        <v>0.71979166666666605</v>
+      </c>
+      <c r="N11">
+        <v>0.171875</v>
+      </c>
+      <c r="O11">
+        <v>0.21354166666666599</v>
       </c>
       <c r="P11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -1033,10 +1032,10 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
         <v>8</v>
@@ -1051,57 +1050,57 @@
         <v>12</v>
       </c>
       <c r="H12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I12" t="s">
         <v>10</v>
       </c>
       <c r="J12">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="K12" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="L12">
-        <v>0.90625</v>
+        <v>0.80625000000000002</v>
       </c>
       <c r="M12">
-        <v>0.89687499999999998</v>
-      </c>
-      <c r="N12" s="1">
-        <v>0.44791666666666602</v>
-      </c>
-      <c r="O12" s="1">
-        <v>0.4375</v>
+        <v>0.81458333333333299</v>
+      </c>
+      <c r="N12">
+        <v>0.140625</v>
+      </c>
+      <c r="O12">
+        <v>0.1875</v>
       </c>
       <c r="P12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" t="s">
-        <v>32</v>
       </c>
       <c r="I13" t="s">
         <v>10</v>
@@ -1110,48 +1109,45 @@
         <v>50</v>
       </c>
       <c r="K13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="L13">
-        <v>0.86595394736842102</v>
+        <v>0.84548611111111105</v>
       </c>
       <c r="M13">
-        <v>0.86019736842105199</v>
+        <v>0.8828125</v>
       </c>
       <c r="N13">
-        <v>3.2894736842105199E-2</v>
+        <v>0.25</v>
       </c>
       <c r="O13">
-        <v>3.94736842105263E-2</v>
-      </c>
-      <c r="P13" t="s">
+        <v>0.296875</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" t="s">
-        <v>32</v>
       </c>
       <c r="I14" t="s">
         <v>10</v>
@@ -1160,10 +1156,22 @@
         <v>50</v>
       </c>
       <c r="K14" t="s">
-        <v>39</v>
+        <v>33</v>
+      </c>
+      <c r="L14">
+        <v>0.59548611111111105</v>
+      </c>
+      <c r="M14">
+        <v>0.59548611111111105</v>
+      </c>
+      <c r="N14">
+        <v>0.171875</v>
+      </c>
+      <c r="O14">
+        <v>0.265625</v>
       </c>
       <c r="P14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -1171,10 +1179,10 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="D15" t="s">
         <v>8</v>
@@ -1198,22 +1206,151 @@
         <v>50</v>
       </c>
       <c r="K15" t="s">
+        <v>33</v>
+      </c>
+      <c r="L15">
+        <v>0.90625</v>
+      </c>
+      <c r="M15">
+        <v>0.89687499999999998</v>
+      </c>
+      <c r="N15" s="1">
+        <v>0.44791666666666602</v>
+      </c>
+      <c r="O15" s="1">
+        <v>0.4375</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>34</v>
       </c>
-      <c r="L15">
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" t="s">
+        <v>10</v>
+      </c>
+      <c r="J16">
+        <v>50</v>
+      </c>
+      <c r="K16" t="s">
+        <v>35</v>
+      </c>
+      <c r="L16">
+        <v>0.86595394736842102</v>
+      </c>
+      <c r="M16">
+        <v>0.86019736842105199</v>
+      </c>
+      <c r="N16">
+        <v>3.2894736842105199E-2</v>
+      </c>
+      <c r="O16">
+        <v>3.94736842105263E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" t="s">
+        <v>31</v>
+      </c>
+      <c r="I17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J17">
+        <v>50</v>
+      </c>
+      <c r="K17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" t="s">
+        <v>10</v>
+      </c>
+      <c r="J18">
+        <v>50</v>
+      </c>
+      <c r="K18" t="s">
+        <v>33</v>
+      </c>
+      <c r="L18">
         <v>0.90798611111111105</v>
       </c>
-      <c r="M15">
+      <c r="M18">
         <v>0.90885416666666596</v>
       </c>
-      <c r="N15" s="2">
+      <c r="N18">
         <v>1.5625E-2</v>
       </c>
-      <c r="O15" s="2">
-        <v>0</v>
-      </c>
-      <c r="P15" t="s">
-        <v>40</v>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
been working on clip_openai script for compute-canada
</commit_message>
<xml_diff>
--- a/CLIP Model Results.xlsx
+++ b/CLIP Model Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Portable\Documents\GitHub\CMPUT624_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harrison\Documents\GitHub\CMPUT624_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09977C0C-F200-4AF5-A708-125BA87F3AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B638A0E-9D3A-4DAA-ABAD-8564D6693AF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="57">
   <si>
     <t>Text Input</t>
   </si>
@@ -148,6 +148,54 @@
   </si>
   <si>
     <t>3D fMRI image 8 seconds after 4th words</t>
+  </si>
+  <si>
+    <t>1-7 (training), 0 (testing)</t>
+  </si>
+  <si>
+    <t>3D fMRI image 4 seconds after last word</t>
+  </si>
+  <si>
+    <t>embed_dim=1024, image_resolution, layers=(2,2,2,2), width=64, context_length=24, vocab_size, transformer_width, transformer_heads, transformer_layers</t>
+  </si>
+  <si>
+    <t>LR=1e-5, batch_size=32, weight_decay=0.2</t>
+  </si>
+  <si>
+    <t>700/0/100</t>
+  </si>
+  <si>
+    <t>slurm-42245994</t>
+  </si>
+  <si>
+    <t>slurm-42257491</t>
+  </si>
+  <si>
+    <t>(Averaged over all subjects) 3D fMRI image 4 seconds after last word</t>
+  </si>
+  <si>
+    <t>(Averaged over all subjects) (detrended) gaussian weighted 3D fMRI image 2-8 seconds after each word</t>
+  </si>
+  <si>
+    <t>slurm-42261175</t>
+  </si>
+  <si>
+    <t>slurm-42263147</t>
+  </si>
+  <si>
+    <t>slurm-42263522</t>
+  </si>
+  <si>
+    <t>slurm-42263524</t>
+  </si>
+  <si>
+    <t>embed_dim=1024, image_resolution, layers=(2,2,2,2), width=64, context_length=48, vocab_size, transformer_width, transformer_heads, transformer_layers</t>
+  </si>
+  <si>
+    <t>(Averaged over all subjects) 3D fMRI image 6 seconds after last word</t>
+  </si>
+  <si>
+    <t>slurm-42263542</t>
   </si>
 </sst>
 </file>
@@ -474,32 +522,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q18"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.54296875" customWidth="1"/>
+    <col min="3" max="3" width="29.7265625" customWidth="1"/>
+    <col min="4" max="4" width="19.7265625" customWidth="1"/>
+    <col min="5" max="5" width="19.81640625" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="32.140625" customWidth="1"/>
-    <col min="9" max="9" width="38.28515625" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" customWidth="1"/>
-    <col min="12" max="12" width="23.28515625" customWidth="1"/>
-    <col min="13" max="13" width="21.7109375" customWidth="1"/>
-    <col min="14" max="14" width="26.5703125" customWidth="1"/>
-    <col min="15" max="16" width="22.140625" customWidth="1"/>
+    <col min="8" max="8" width="32.1796875" customWidth="1"/>
+    <col min="9" max="9" width="38.26953125" customWidth="1"/>
+    <col min="10" max="10" width="11.26953125" customWidth="1"/>
+    <col min="11" max="11" width="15.26953125" customWidth="1"/>
+    <col min="12" max="12" width="23.26953125" customWidth="1"/>
+    <col min="13" max="13" width="21.7265625" customWidth="1"/>
+    <col min="14" max="14" width="26.54296875" customWidth="1"/>
+    <col min="15" max="16" width="22.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -552,7 +600,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -599,7 +647,7 @@
         <v>3.90625E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>0</v>
       </c>
@@ -646,7 +694,7 @@
         <v>2.34375E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>0</v>
       </c>
@@ -694,7 +742,7 @@
       </c>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>0</v>
       </c>
@@ -742,7 +790,7 @@
       </c>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>0</v>
       </c>
@@ -789,7 +837,7 @@
         <v>3.90625E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>0</v>
       </c>
@@ -836,7 +884,7 @@
         <v>2.34375E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>0</v>
       </c>
@@ -883,7 +931,7 @@
         <v>2.734375E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>0</v>
       </c>
@@ -930,7 +978,7 @@
         <v>3.515625E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>0</v>
       </c>
@@ -977,7 +1025,7 @@
         <v>0.203125</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>0</v>
       </c>
@@ -1027,7 +1075,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>0</v>
       </c>
@@ -1077,7 +1125,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>0</v>
       </c>
@@ -1124,7 +1172,7 @@
         <v>0.296875</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>0</v>
       </c>
@@ -1174,7 +1222,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>0</v>
       </c>
@@ -1221,7 +1269,7 @@
         <v>0.4375</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1268,7 +1316,7 @@
         <v>3.94736842105263E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -1303,7 +1351,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>0</v>
       </c>
@@ -1351,6 +1399,343 @@
       </c>
       <c r="P18" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" t="s">
+        <v>43</v>
+      </c>
+      <c r="I19" t="s">
+        <v>44</v>
+      </c>
+      <c r="J19">
+        <v>100</v>
+      </c>
+      <c r="K19" t="s">
+        <v>45</v>
+      </c>
+      <c r="L19">
+        <v>0.42389838129496399</v>
+      </c>
+      <c r="M19">
+        <v>0.439186151079136</v>
+      </c>
+      <c r="N19">
+        <v>0.11939102564102499</v>
+      </c>
+      <c r="O19">
+        <v>0.13541666666666599</v>
+      </c>
+      <c r="P19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20" t="s">
+        <v>44</v>
+      </c>
+      <c r="J20">
+        <v>100</v>
+      </c>
+      <c r="K20" t="s">
+        <v>45</v>
+      </c>
+      <c r="L20">
+        <v>0.42153776978417201</v>
+      </c>
+      <c r="M20">
+        <v>0.42884442446043097</v>
+      </c>
+      <c r="N20">
+        <v>8.8141025641025605E-2</v>
+      </c>
+      <c r="O20">
+        <v>0.103365384615384</v>
+      </c>
+      <c r="P20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" t="s">
+        <v>31</v>
+      </c>
+      <c r="I21" t="s">
+        <v>44</v>
+      </c>
+      <c r="J21">
+        <v>100</v>
+      </c>
+      <c r="K21" t="s">
+        <v>35</v>
+      </c>
+      <c r="L21">
+        <v>0.99278846153846101</v>
+      </c>
+      <c r="M21">
+        <v>0.98557692307692302</v>
+      </c>
+      <c r="N21">
+        <v>6.5705128205128194E-2</v>
+      </c>
+      <c r="O21">
+        <v>6.6506410256410201E-2</v>
+      </c>
+      <c r="P21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" t="s">
+        <v>26</v>
+      </c>
+      <c r="J22">
+        <v>100</v>
+      </c>
+      <c r="K22" t="s">
+        <v>35</v>
+      </c>
+      <c r="P22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" t="s">
+        <v>43</v>
+      </c>
+      <c r="I23" t="s">
+        <v>44</v>
+      </c>
+      <c r="J23">
+        <v>50</v>
+      </c>
+      <c r="K23" t="s">
+        <v>35</v>
+      </c>
+      <c r="P23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" t="s">
+        <v>43</v>
+      </c>
+      <c r="I24" t="s">
+        <v>44</v>
+      </c>
+      <c r="J24">
+        <v>10</v>
+      </c>
+      <c r="K24" t="s">
+        <v>35</v>
+      </c>
+      <c r="P24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I25" t="s">
+        <v>44</v>
+      </c>
+      <c r="J25">
+        <v>50</v>
+      </c>
+      <c r="K25" t="s">
+        <v>35</v>
+      </c>
+      <c r="P25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" t="s">
+        <v>31</v>
+      </c>
+      <c r="I26" t="s">
+        <v>44</v>
+      </c>
+      <c r="J26">
+        <v>100</v>
+      </c>
+      <c r="K26" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated preprocessing2 to output fmri indices and did more experiments
</commit_message>
<xml_diff>
--- a/CLIP Model Results.xlsx
+++ b/CLIP Model Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harrison\Documents\GitHub\CMPUT624_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Portable\Documents\GitHub\CMPUT624_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6816F59D-3BEB-4250-977A-94471C5C0CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99189F9E-401D-4CDA-962A-B8647A9979A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="122">
   <si>
     <t>Text Input</t>
   </si>
@@ -174,9 +174,6 @@
     <t>(Averaged over all subjects) 3D fMRI image 4 seconds after last word</t>
   </si>
   <si>
-    <t>(Averaged over all subjects) (detrended) gaussian weighted 3D fMRI image 2-8 seconds after each word</t>
-  </si>
-  <si>
     <t>slurm-42261175</t>
   </si>
   <si>
@@ -225,9 +222,6 @@
     <t>(unnormalized) (all samples in a batch belong to one subject) gaussian weighted 3D fMRI image 2-8 seconds after each word</t>
   </si>
   <si>
-    <t>LR=1e-6, batch_size=32, weight_decay=0.2</t>
-  </si>
-  <si>
     <t>slurm-42304386</t>
   </si>
   <si>
@@ -268,6 +262,135 @@
   </si>
   <si>
     <t>slurm-42326017</t>
+  </si>
+  <si>
+    <t>slurm-42355449</t>
+  </si>
+  <si>
+    <t>32 batch and 2 batch accuracies</t>
+  </si>
+  <si>
+    <t>slurm-42355485</t>
+  </si>
+  <si>
+    <t>32 batch: 0.9103794642857143, 2 batch: 0.938823267216403</t>
+  </si>
+  <si>
+    <t>32 batch: 0.8571428571428571, 2 batch: 0.9602184087363494</t>
+  </si>
+  <si>
+    <t>32 batch: 0.11875, 2 batch: 0.6684867394695788</t>
+  </si>
+  <si>
+    <t>32 batch: 0.1171875, 2 batch: 0.6739469578783152</t>
+  </si>
+  <si>
+    <t>0.93046875, 0.932142857142857, 0.9338169642857143, 0.9438616071428572, 0.9302455357142857, 0.9385044642857143, 0.9417410714285714, 0.9286830357142857</t>
+  </si>
+  <si>
+    <t>0.9194196428571428, 0.910379464285714, 0.9193080357142858, 0.9285714285714286, 0.9176339285714286, 0.9194196428571428, 0.9241071428571429, 0.9053571428571429</t>
+  </si>
+  <si>
+    <t>0.08203125, 0.096875, 0.13515625, 0.06484375, 0.03984375, 0.08125, 0.08671875, 0.09296875</t>
+  </si>
+  <si>
+    <t>0.08515625, 0.10078125, 0.1359375, 0.06875, 0.02890625, 0.08359375, 0.07265625, 0.08359375</t>
+  </si>
+  <si>
+    <t>0.927901785714285, 0.9388392857142858, 0.9448660714285714, 0.9459821428571429, 0.9498883928571429, 0.9542410714285714, 0.9457589285714286, 0.9339285714285714</t>
+  </si>
+  <si>
+    <t>0.918526785714285, 0.91484375, 0.9204241071428572, 0.9254464285714286, 0.9371651785714286, 0.9409598214285714, 0.91875, 0.9142857142857143</t>
+  </si>
+  <si>
+    <t>0.075, 0.0734375, 0.1, 0.09765625, 0.071875, 0.04765625, 0.0796875, 0.1078125</t>
+  </si>
+  <si>
+    <t>0.075, 0.07421875, 0.09140625, 0.0921875, 0.05625, 0.06171875, 0.0921875, 0.096875</t>
+  </si>
+  <si>
+    <t>0.956473214285714, 0.9696428571428571</t>
+  </si>
+  <si>
+    <t>0.933816964285714, 0.9505580357142858</t>
+  </si>
+  <si>
+    <t>0.121875, 0.11015625</t>
+  </si>
+  <si>
+    <t>0.13828125, 0.1078125</t>
+  </si>
+  <si>
+    <t>32 batch: 0.1109375, 2 batch: 0.6583463338533542</t>
+  </si>
+  <si>
+    <t>32 batch: 0.09921875, 2 batch: 0.6747269890795632</t>
+  </si>
+  <si>
+    <t>32 batch: 0.9053571428571429, 2 batch: 0.9365946066414085</t>
+  </si>
+  <si>
+    <t>32 batch: 0.85234375, 2 batch: 0.9611098729663472</t>
+  </si>
+  <si>
+    <t>subj 1, 2 leave-one-out average</t>
+  </si>
+  <si>
+    <t>Untrained model</t>
+  </si>
+  <si>
+    <t>Random model</t>
+  </si>
+  <si>
+    <t>(detrended) gaussian weighted 3D fMRI image 2-8 seconds after each word</t>
+  </si>
+  <si>
+    <t>slurm-42368858</t>
+  </si>
+  <si>
+    <t>slurm-42383209</t>
+  </si>
+  <si>
+    <t>32 batch: 0.030245535714285714, 2 batch: 0.5003342990862492</t>
+  </si>
+  <si>
+    <t>32 batch: 0.034375, 2 batch: 0.5037887229774906</t>
+  </si>
+  <si>
+    <t>32 batch: 0.03125, 2 batch: 0.516380655226209</t>
+  </si>
+  <si>
+    <t>32 batch: 0.0281251, 2 batch: 0.5015600624024961</t>
+  </si>
+  <si>
+    <t>32 batch: 0.03046875, 2 batch: 0.4988856697125028</t>
+  </si>
+  <si>
+    <t>32 batch: 0.032589285714285716, 2 batch: 0.4974370403387564</t>
+  </si>
+  <si>
+    <t>32 batch: 0.02578125, 2 batch: 0.5039001560062403</t>
+  </si>
+  <si>
+    <t>32 batch: 0.0375, 2 batch: 0.48517940717628705</t>
+  </si>
+  <si>
+    <t>32 batch: 0.93828125, 2 batch: 0.959215511477602</t>
+  </si>
+  <si>
+    <t>32 batch: 0.8886160714285715, 2 batch: 0.9706931134388233</t>
+  </si>
+  <si>
+    <t>32 batch: 0.09609375, 2 batch: 0.65600624024961</t>
+  </si>
+  <si>
+    <t>32 batch: 0.09921875, 2 batch: 0.6700468018720749</t>
+  </si>
+  <si>
+    <t>(detrended with rests) gaussian weighted 3D fMRI image 2-8 seconds after each word</t>
+  </si>
+  <si>
+    <t>slurm-42386935</t>
   </si>
 </sst>
 </file>
@@ -311,9 +434,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,32 +720,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q45"/>
+  <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K32" workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+    <sheetView tabSelected="1" topLeftCell="E22" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="14.54296875" customWidth="1"/>
-    <col min="3" max="3" width="29.7265625" customWidth="1"/>
-    <col min="4" max="4" width="19.7265625" customWidth="1"/>
-    <col min="5" max="5" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="32.1796875" customWidth="1"/>
-    <col min="9" max="9" width="38.26953125" customWidth="1"/>
-    <col min="10" max="10" width="11.26953125" customWidth="1"/>
-    <col min="11" max="11" width="15.26953125" customWidth="1"/>
-    <col min="12" max="12" width="23.26953125" customWidth="1"/>
-    <col min="13" max="13" width="21.7265625" customWidth="1"/>
-    <col min="14" max="14" width="26.54296875" customWidth="1"/>
-    <col min="15" max="16" width="22.1796875" customWidth="1"/>
+    <col min="8" max="8" width="32.140625" customWidth="1"/>
+    <col min="9" max="9" width="38.28515625" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" customWidth="1"/>
+    <col min="12" max="12" width="23.28515625" customWidth="1"/>
+    <col min="13" max="13" width="21.7109375" customWidth="1"/>
+    <col min="14" max="14" width="26.5703125" customWidth="1"/>
+    <col min="15" max="16" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -672,7 +798,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -719,7 +845,7 @@
         <v>3.90625E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -766,7 +892,7 @@
         <v>2.34375E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -814,7 +940,7 @@
       </c>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -862,7 +988,7 @@
       </c>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -909,7 +1035,7 @@
         <v>3.90625E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -956,7 +1082,7 @@
         <v>2.34375E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -1003,7 +1129,7 @@
         <v>2.734375E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -1050,7 +1176,7 @@
         <v>3.515625E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -1097,7 +1223,7 @@
         <v>0.203125</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0</v>
       </c>
@@ -1147,7 +1273,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -1197,7 +1323,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
@@ -1244,7 +1370,7 @@
         <v>0.296875</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -1294,7 +1420,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -1341,7 +1467,7 @@
         <v>0.4375</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1388,7 +1514,7 @@
         <v>3.94736842105263E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -1423,7 +1549,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0</v>
       </c>
@@ -1473,7 +1599,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -1523,7 +1649,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>41</v>
       </c>
@@ -1573,7 +1699,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -1620,10 +1746,10 @@
         <v>6.6506410256410201E-2</v>
       </c>
       <c r="P21" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -1670,10 +1796,10 @@
         <v>8.9743589743589702E-2</v>
       </c>
       <c r="P22" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -1720,10 +1846,10 @@
         <v>5.4487179487179398E-2</v>
       </c>
       <c r="P23" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -1770,10 +1896,10 @@
         <v>8.5737179487179405E-2</v>
       </c>
       <c r="P24" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -1781,7 +1907,7 @@
         <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D25" t="s">
         <v>8</v>
@@ -1796,7 +1922,7 @@
         <v>12</v>
       </c>
       <c r="H25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I25" t="s">
         <v>44</v>
@@ -1820,10 +1946,10 @@
         <v>6.4903846153846104E-2</v>
       </c>
       <c r="P25" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -1831,7 +1957,7 @@
         <v>28</v>
       </c>
       <c r="C26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D26" t="s">
         <v>8</v>
@@ -1846,7 +1972,7 @@
         <v>12</v>
       </c>
       <c r="H26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I26" t="s">
         <v>44</v>
@@ -1870,10 +1996,10 @@
         <v>9.6153846153846104E-2</v>
       </c>
       <c r="P26" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -1881,7 +2007,7 @@
         <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D27" t="s">
         <v>8</v>
@@ -1896,7 +2022,7 @@
         <v>12</v>
       </c>
       <c r="H27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I27" t="s">
         <v>44</v>
@@ -1920,10 +2046,10 @@
         <v>8.9743589743589702E-2</v>
       </c>
       <c r="P27" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -1931,7 +2057,7 @@
         <v>28</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D28" t="s">
         <v>8</v>
@@ -1946,7 +2072,7 @@
         <v>12</v>
       </c>
       <c r="H28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I28" t="s">
         <v>44</v>
@@ -1970,10 +2096,10 @@
         <v>7.4519230769230699E-2</v>
       </c>
       <c r="P28" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -1981,7 +2107,7 @@
         <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D29" t="s">
         <v>8</v>
@@ -2020,10 +2146,10 @@
         <v>6.7187499999999997E-2</v>
       </c>
       <c r="P29" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -2031,7 +2157,7 @@
         <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D30" t="s">
         <v>8</v>
@@ -2070,10 +2196,10 @@
         <v>9.1406249999999994E-2</v>
       </c>
       <c r="P30" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -2081,7 +2207,7 @@
         <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D31" t="s">
         <v>8</v>
@@ -2120,10 +2246,10 @@
         <v>0.10781250000000001</v>
       </c>
       <c r="P31" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -2131,7 +2257,7 @@
         <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D32" t="s">
         <v>8</v>
@@ -2170,10 +2296,10 @@
         <v>0.10390625000000001</v>
       </c>
       <c r="P32" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -2181,7 +2307,7 @@
         <v>6</v>
       </c>
       <c r="C33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D33" t="s">
         <v>8</v>
@@ -2220,10 +2346,10 @@
         <v>0.10234375</v>
       </c>
       <c r="P33" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -2231,7 +2357,7 @@
         <v>6</v>
       </c>
       <c r="C34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D34" t="s">
         <v>8</v>
@@ -2270,10 +2396,10 @@
         <v>0.10703124999999999</v>
       </c>
       <c r="P34" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -2281,7 +2407,7 @@
         <v>24</v>
       </c>
       <c r="C35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D35" t="s">
         <v>8</v>
@@ -2320,10 +2446,10 @@
         <v>0.13671875</v>
       </c>
       <c r="P35" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -2331,7 +2457,7 @@
         <v>28</v>
       </c>
       <c r="C36" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D36" t="s">
         <v>8</v>
@@ -2370,10 +2496,10 @@
         <v>9.7756410256410201E-2</v>
       </c>
       <c r="P36" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -2381,7 +2507,7 @@
         <v>6</v>
       </c>
       <c r="C37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D37" t="s">
         <v>8</v>
@@ -2420,10 +2546,10 @@
         <v>7.03125E-2</v>
       </c>
       <c r="P37" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -2431,7 +2557,7 @@
         <v>24</v>
       </c>
       <c r="C38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D38" t="s">
         <v>8</v>
@@ -2457,11 +2583,23 @@
       <c r="K38" t="s">
         <v>45</v>
       </c>
+      <c r="L38">
+        <v>0.34006696428571398</v>
+      </c>
+      <c r="M38">
+        <v>0.32857142857142801</v>
+      </c>
+      <c r="N38">
+        <v>0.10703124999999999</v>
+      </c>
+      <c r="O38">
+        <v>9.8437499999999997E-2</v>
+      </c>
       <c r="P38" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -2469,7 +2607,7 @@
         <v>24</v>
       </c>
       <c r="C39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D39" t="s">
         <v>8</v>
@@ -2490,24 +2628,36 @@
         <v>44</v>
       </c>
       <c r="J39">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="K39" t="s">
         <v>45</v>
       </c>
+      <c r="L39" t="s">
+        <v>100</v>
+      </c>
+      <c r="M39" t="s">
+        <v>101</v>
+      </c>
+      <c r="N39" t="s">
+        <v>98</v>
+      </c>
+      <c r="O39" t="s">
+        <v>99</v>
+      </c>
       <c r="P39" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="B40" t="s">
         <v>24</v>
       </c>
       <c r="C40" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D40" t="s">
         <v>8</v>
@@ -2525,7 +2675,7 @@
         <v>22</v>
       </c>
       <c r="I40" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="J40">
         <v>100</v>
@@ -2533,24 +2683,81 @@
       <c r="K40" t="s">
         <v>45</v>
       </c>
+      <c r="L40" t="s">
+        <v>86</v>
+      </c>
+      <c r="M40" t="s">
+        <v>87</v>
+      </c>
+      <c r="N40" t="s">
+        <v>88</v>
+      </c>
+      <c r="O40" t="s">
+        <v>89</v>
+      </c>
       <c r="P40" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" t="s">
+        <v>24</v>
+      </c>
       <c r="C41" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="D41" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" t="s">
+        <v>8</v>
+      </c>
+      <c r="F41" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41" t="s">
+        <v>12</v>
+      </c>
+      <c r="H41" t="s">
+        <v>21</v>
+      </c>
+      <c r="I41" t="s">
+        <v>44</v>
+      </c>
+      <c r="J41">
+        <v>100</v>
+      </c>
+      <c r="K41" t="s">
+        <v>45</v>
+      </c>
+      <c r="L41" t="s">
+        <v>90</v>
+      </c>
+      <c r="M41" t="s">
+        <v>91</v>
+      </c>
+      <c r="N41" t="s">
+        <v>92</v>
+      </c>
+      <c r="O41" t="s">
+        <v>93</v>
+      </c>
+      <c r="P41" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>24</v>
       </c>
       <c r="C42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D42" t="s">
         <v>8</v>
@@ -2565,7 +2772,7 @@
         <v>12</v>
       </c>
       <c r="H42" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I42" t="s">
         <v>44</v>
@@ -2576,21 +2783,31 @@
       <c r="K42" t="s">
         <v>45</v>
       </c>
-      <c r="N42" s="1"/>
-      <c r="O42" s="1"/>
+      <c r="L42">
+        <v>0.96863839285714204</v>
+      </c>
+      <c r="M42">
+        <v>0.94341517857142798</v>
+      </c>
+      <c r="N42">
+        <v>9.765625E-2</v>
+      </c>
+      <c r="O42">
+        <v>0.109375</v>
+      </c>
       <c r="P42" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="B43" t="s">
         <v>24</v>
       </c>
       <c r="C43" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D43" t="s">
         <v>8</v>
@@ -2605,7 +2822,7 @@
         <v>12</v>
       </c>
       <c r="H43" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="I43" t="s">
         <v>44</v>
@@ -2616,11 +2833,23 @@
       <c r="K43" t="s">
         <v>45</v>
       </c>
+      <c r="L43" t="s">
+        <v>94</v>
+      </c>
+      <c r="M43" t="s">
+        <v>95</v>
+      </c>
+      <c r="N43" t="s">
+        <v>96</v>
+      </c>
+      <c r="O43" t="s">
+        <v>97</v>
+      </c>
       <c r="P43" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>41</v>
       </c>
@@ -2628,7 +2857,7 @@
         <v>24</v>
       </c>
       <c r="C44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D44" t="s">
         <v>8</v>
@@ -2643,22 +2872,37 @@
         <v>12</v>
       </c>
       <c r="H44" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I44" t="s">
         <v>44</v>
       </c>
       <c r="J44">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="K44" t="s">
         <v>45</v>
       </c>
+      <c r="L44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M44" t="s">
+        <v>83</v>
+      </c>
+      <c r="N44" t="s">
+        <v>84</v>
+      </c>
+      <c r="O44" t="s">
+        <v>85</v>
+      </c>
       <c r="P44" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>41</v>
       </c>
@@ -2666,7 +2910,7 @@
         <v>24</v>
       </c>
       <c r="C45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D45" t="s">
         <v>8</v>
@@ -2681,19 +2925,139 @@
         <v>12</v>
       </c>
       <c r="H45" t="s">
-        <v>79</v>
+        <v>22</v>
       </c>
       <c r="I45" t="s">
         <v>44</v>
       </c>
       <c r="J45">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="K45" t="s">
         <v>45</v>
       </c>
+      <c r="L45" t="s">
+        <v>108</v>
+      </c>
+      <c r="M45" t="s">
+        <v>109</v>
+      </c>
+      <c r="N45" t="s">
+        <v>110</v>
+      </c>
+      <c r="O45" s="2" t="s">
+        <v>111</v>
+      </c>
       <c r="P45" t="s">
-        <v>80</v>
+        <v>106</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L46" t="s">
+        <v>112</v>
+      </c>
+      <c r="M46" t="s">
+        <v>113</v>
+      </c>
+      <c r="N46" t="s">
+        <v>114</v>
+      </c>
+      <c r="O46" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" t="s">
+        <v>120</v>
+      </c>
+      <c r="D47" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" t="s">
+        <v>9</v>
+      </c>
+      <c r="G47" t="s">
+        <v>12</v>
+      </c>
+      <c r="H47" t="s">
+        <v>22</v>
+      </c>
+      <c r="I47" t="s">
+        <v>44</v>
+      </c>
+      <c r="J47">
+        <v>100</v>
+      </c>
+      <c r="K47" t="s">
+        <v>45</v>
+      </c>
+      <c r="L47" t="s">
+        <v>116</v>
+      </c>
+      <c r="M47" t="s">
+        <v>117</v>
+      </c>
+      <c r="N47" t="s">
+        <v>118</v>
+      </c>
+      <c r="O47" t="s">
+        <v>119</v>
+      </c>
+      <c r="P47" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B48" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" t="s">
+        <v>105</v>
+      </c>
+      <c r="D48" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" t="s">
+        <v>8</v>
+      </c>
+      <c r="F48" t="s">
+        <v>9</v>
+      </c>
+      <c r="G48" t="s">
+        <v>12</v>
+      </c>
+      <c r="H48" t="s">
+        <v>22</v>
+      </c>
+      <c r="I48" t="s">
+        <v>44</v>
+      </c>
+      <c r="J48">
+        <v>100</v>
+      </c>
+      <c r="K48" t="s">
+        <v>45</v>
+      </c>
+      <c r="P48" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated clip model results
</commit_message>
<xml_diff>
--- a/CLIP Model Results.xlsx
+++ b/CLIP Model Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harrison\Documents\GitHub\CMPUT624_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01DB00F1-9466-4AF9-8657-E05F18FB582D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E7B3AF-AF17-4B48-8450-CD4D92389A74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="155">
   <si>
     <t>Text Input</t>
   </si>
@@ -405,10 +405,91 @@
     <t>32 batch: 0.07154605263157894, 2 batch: 0.6079545454545454</t>
   </si>
   <si>
-    <t xml:space="preserve">32 batch: , 2 batch: </t>
-  </si>
-  <si>
     <t>slurm-42391225</t>
+  </si>
+  <si>
+    <t>32 batch: 0.9611137218045113, 2 batch: 0.9399906781635983</t>
+  </si>
+  <si>
+    <t>32 batch: 0.9464285714285714, 2 batch: 0.958168259147052</t>
+  </si>
+  <si>
+    <t>32 batch: 0.08223684210526316, 2 batch: 0.6313213703099511</t>
+  </si>
+  <si>
+    <t>32 batch: 0.08634868421052631, 2 batch: 0.636215334420881</t>
+  </si>
+  <si>
+    <t>slurm-42396686</t>
+  </si>
+  <si>
+    <t>LR=5e-4, batch_size=32, weight_decay=0.2</t>
+  </si>
+  <si>
+    <t>LR=5e-5, batch_size=32, weight_decay=0.2</t>
+  </si>
+  <si>
+    <t>32 batch: 0.03125, 2 batch: 0.5</t>
+  </si>
+  <si>
+    <t>32 batch: 0.9459586466165414, 2 batch: 0.9461663947797716</t>
+  </si>
+  <si>
+    <t>32 batch: 0.930921052631579, 2 batch: 0.9550221393614542</t>
+  </si>
+  <si>
+    <t>32 batch: 0.07072368421052631, 2 batch: 0.5628058727569332</t>
+  </si>
+  <si>
+    <t>32 batch: 0.0625, 2 batch: 0.5497553017944535</t>
+  </si>
+  <si>
+    <t>32 batch: 0.7095864661654135, 2 batch: 0.9591004427872291</t>
+  </si>
+  <si>
+    <t>32 batch: 0.6766917293233082, 2 batch: 0.9882311815427639</t>
+  </si>
+  <si>
+    <t>32 batch: 0.10032894736842106, 2 batch: 0.6419249592169658</t>
+  </si>
+  <si>
+    <t>32 batch: 0.09046052631578948, 2 batch</t>
+  </si>
+  <si>
+    <t>LR=1e-5, batch_size=64, weight_decay=0.2</t>
+  </si>
+  <si>
+    <t>LR=5e-5, batch_size=64, weight_decay=0.2</t>
+  </si>
+  <si>
+    <t>slurm-42435618</t>
+  </si>
+  <si>
+    <t>64 batch: 0.945371240601503, 2 batch: 0.9108599394080634</t>
+  </si>
+  <si>
+    <t>64 batch: 0.9273966165413534, 2 batch: 0.9535073409461664</t>
+  </si>
+  <si>
+    <t>64 batch: 0.017269736842105265, 2 batch: 0.586460032626427</t>
+  </si>
+  <si>
+    <t>64 batch: 0.02631578947368421, 2 batch: 0.6117455138662317</t>
+  </si>
+  <si>
+    <t>64 batch: 0.543233082706767, 2 batch: 0.9364949895129341</t>
+  </si>
+  <si>
+    <t>64 batch: 0.5110432330827067, 2 batch: 0.97657888604055</t>
+  </si>
+  <si>
+    <t>64 batch: 0.05674342105263158, 2 batch: 0.6786296900489397</t>
+  </si>
+  <si>
+    <t>64 batch: 0.0805921052631579, 2 batch: 0.7047308319738989</t>
+  </si>
+  <si>
+    <t>(fmri channel for each word) (detrended) gaussian weighted 3D fMRI image 2-8 seconds after each word</t>
   </si>
 </sst>
 </file>
@@ -738,10 +819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q49"/>
+  <dimension ref="A1:Q55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I41" workbookViewId="0">
-      <selection activeCell="L45" sqref="L45"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3125,19 +3206,274 @@
         <v>45</v>
       </c>
       <c r="L49" t="s">
+        <v>127</v>
+      </c>
+      <c r="M49" t="s">
+        <v>128</v>
+      </c>
+      <c r="N49" t="s">
+        <v>129</v>
+      </c>
+      <c r="O49" t="s">
+        <v>130</v>
+      </c>
+      <c r="P49" t="s">
         <v>126</v>
       </c>
-      <c r="M49" t="s">
-        <v>126</v>
-      </c>
-      <c r="N49" t="s">
-        <v>126</v>
-      </c>
-      <c r="O49" t="s">
-        <v>126</v>
-      </c>
-      <c r="P49" t="s">
-        <v>127</v>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>41</v>
+      </c>
+      <c r="B50" t="s">
+        <v>28</v>
+      </c>
+      <c r="C50" t="s">
+        <v>105</v>
+      </c>
+      <c r="D50" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" t="s">
+        <v>8</v>
+      </c>
+      <c r="F50" t="s">
+        <v>9</v>
+      </c>
+      <c r="G50" t="s">
+        <v>12</v>
+      </c>
+      <c r="H50" t="s">
+        <v>21</v>
+      </c>
+      <c r="I50" t="s">
+        <v>132</v>
+      </c>
+      <c r="J50">
+        <v>100</v>
+      </c>
+      <c r="K50" t="s">
+        <v>45</v>
+      </c>
+      <c r="L50" t="s">
+        <v>134</v>
+      </c>
+      <c r="M50" t="s">
+        <v>134</v>
+      </c>
+      <c r="N50" t="s">
+        <v>134</v>
+      </c>
+      <c r="O50" t="s">
+        <v>134</v>
+      </c>
+      <c r="P50" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>41</v>
+      </c>
+      <c r="B51" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51" t="s">
+        <v>105</v>
+      </c>
+      <c r="D51" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" t="s">
+        <v>8</v>
+      </c>
+      <c r="F51" t="s">
+        <v>9</v>
+      </c>
+      <c r="G51" t="s">
+        <v>12</v>
+      </c>
+      <c r="H51" t="s">
+        <v>21</v>
+      </c>
+      <c r="I51" t="s">
+        <v>44</v>
+      </c>
+      <c r="J51">
+        <v>100</v>
+      </c>
+      <c r="K51" t="s">
+        <v>45</v>
+      </c>
+      <c r="L51" t="s">
+        <v>135</v>
+      </c>
+      <c r="M51" t="s">
+        <v>136</v>
+      </c>
+      <c r="N51" t="s">
+        <v>137</v>
+      </c>
+      <c r="O51" t="s">
+        <v>138</v>
+      </c>
+      <c r="P51" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>41</v>
+      </c>
+      <c r="B52" t="s">
+        <v>28</v>
+      </c>
+      <c r="C52" t="s">
+        <v>105</v>
+      </c>
+      <c r="D52" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" t="s">
+        <v>8</v>
+      </c>
+      <c r="F52" t="s">
+        <v>9</v>
+      </c>
+      <c r="G52" t="s">
+        <v>12</v>
+      </c>
+      <c r="H52" t="s">
+        <v>21</v>
+      </c>
+      <c r="I52" t="s">
+        <v>133</v>
+      </c>
+      <c r="J52">
+        <v>100</v>
+      </c>
+      <c r="K52" t="s">
+        <v>45</v>
+      </c>
+      <c r="L52" t="s">
+        <v>139</v>
+      </c>
+      <c r="M52" t="s">
+        <v>140</v>
+      </c>
+      <c r="N52" t="s">
+        <v>141</v>
+      </c>
+      <c r="O52" t="s">
+        <v>142</v>
+      </c>
+      <c r="P52" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>41</v>
+      </c>
+      <c r="B53" t="s">
+        <v>28</v>
+      </c>
+      <c r="C53" t="s">
+        <v>105</v>
+      </c>
+      <c r="D53" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" t="s">
+        <v>8</v>
+      </c>
+      <c r="F53" t="s">
+        <v>9</v>
+      </c>
+      <c r="G53" t="s">
+        <v>12</v>
+      </c>
+      <c r="H53" t="s">
+        <v>22</v>
+      </c>
+      <c r="I53" t="s">
+        <v>143</v>
+      </c>
+      <c r="J53">
+        <v>100</v>
+      </c>
+      <c r="K53" t="s">
+        <v>45</v>
+      </c>
+      <c r="L53" t="s">
+        <v>146</v>
+      </c>
+      <c r="M53" t="s">
+        <v>147</v>
+      </c>
+      <c r="N53" t="s">
+        <v>148</v>
+      </c>
+      <c r="O53" t="s">
+        <v>149</v>
+      </c>
+      <c r="P53" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>41</v>
+      </c>
+      <c r="B54" t="s">
+        <v>28</v>
+      </c>
+      <c r="C54" t="s">
+        <v>105</v>
+      </c>
+      <c r="D54" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54" t="s">
+        <v>8</v>
+      </c>
+      <c r="F54" t="s">
+        <v>9</v>
+      </c>
+      <c r="G54" t="s">
+        <v>12</v>
+      </c>
+      <c r="H54" t="s">
+        <v>22</v>
+      </c>
+      <c r="I54" t="s">
+        <v>144</v>
+      </c>
+      <c r="J54">
+        <v>100</v>
+      </c>
+      <c r="K54" t="s">
+        <v>45</v>
+      </c>
+      <c r="L54" t="s">
+        <v>150</v>
+      </c>
+      <c r="M54" t="s">
+        <v>151</v>
+      </c>
+      <c r="N54" t="s">
+        <v>152</v>
+      </c>
+      <c r="O54" t="s">
+        <v>153</v>
+      </c>
+      <c r="P54" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="C55" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wrote file for computing individual word fmris
</commit_message>
<xml_diff>
--- a/CLIP Model Results.xlsx
+++ b/CLIP Model Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harrison\Documents\GitHub\CMPUT624_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Portable\Documents\GitHub\CMPUT624_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E7B3AF-AF17-4B48-8450-CD4D92389A74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706C5865-90DC-4887-8FDF-B10A7F097047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="155">
   <si>
     <t>Text Input</t>
   </si>
@@ -819,32 +819,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q55"/>
+  <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="E45" workbookViewId="0">
+      <selection activeCell="P56" sqref="P56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="14.54296875" customWidth="1"/>
-    <col min="3" max="3" width="29.7265625" customWidth="1"/>
-    <col min="4" max="4" width="19.7265625" customWidth="1"/>
-    <col min="5" max="5" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="32.1796875" customWidth="1"/>
-    <col min="9" max="9" width="38.26953125" customWidth="1"/>
-    <col min="10" max="10" width="11.26953125" customWidth="1"/>
-    <col min="11" max="11" width="15.26953125" customWidth="1"/>
-    <col min="12" max="12" width="23.26953125" customWidth="1"/>
-    <col min="13" max="13" width="21.7265625" customWidth="1"/>
-    <col min="14" max="14" width="26.54296875" customWidth="1"/>
-    <col min="15" max="16" width="22.1796875" customWidth="1"/>
+    <col min="8" max="8" width="32.140625" customWidth="1"/>
+    <col min="9" max="9" width="38.28515625" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" customWidth="1"/>
+    <col min="12" max="12" width="23.28515625" customWidth="1"/>
+    <col min="13" max="13" width="21.7109375" customWidth="1"/>
+    <col min="14" max="14" width="26.5703125" customWidth="1"/>
+    <col min="15" max="16" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -897,7 +897,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -944,7 +944,7 @@
         <v>3.90625E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -991,7 +991,7 @@
         <v>2.34375E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1039,7 +1039,7 @@
       </c>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -1134,7 +1134,7 @@
         <v>3.90625E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -1181,7 +1181,7 @@
         <v>2.34375E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>2.734375E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -1275,7 +1275,7 @@
         <v>3.515625E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>0.203125</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>0.296875</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -1519,7 +1519,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>0.4375</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>3.94736842105263E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>41</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -1898,7 +1898,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -1948,7 +1948,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -2048,7 +2048,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -2148,7 +2148,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -2348,7 +2348,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -2448,7 +2448,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -2498,7 +2498,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -2548,7 +2548,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -2598,7 +2598,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -2648,7 +2648,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -2698,7 +2698,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -2748,7 +2748,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>72</v>
       </c>
@@ -2798,7 +2798,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>72</v>
       </c>
@@ -2848,7 +2848,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -2898,7 +2898,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>102</v>
       </c>
@@ -2948,7 +2948,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>41</v>
       </c>
@@ -3001,7 +3001,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>41</v>
       </c>
@@ -3054,7 +3054,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="L46" t="s">
         <v>112</v>
       </c>
@@ -3071,7 +3071,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>41</v>
       </c>
@@ -3121,7 +3121,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>41</v>
       </c>
@@ -3171,7 +3171,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>41</v>
       </c>
@@ -3221,7 +3221,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>41</v>
       </c>
@@ -3271,7 +3271,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>41</v>
       </c>
@@ -3321,7 +3321,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>41</v>
       </c>
@@ -3371,7 +3371,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>41</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>41</v>
       </c>
@@ -3471,9 +3471,74 @@
         <v>145</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>41</v>
+      </c>
+      <c r="B55" t="s">
+        <v>6</v>
+      </c>
       <c r="C55" t="s">
         <v>154</v>
+      </c>
+      <c r="D55" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" t="s">
+        <v>8</v>
+      </c>
+      <c r="F55" t="s">
+        <v>9</v>
+      </c>
+      <c r="G55" t="s">
+        <v>12</v>
+      </c>
+      <c r="H55" t="s">
+        <v>22</v>
+      </c>
+      <c r="I55" t="s">
+        <v>44</v>
+      </c>
+      <c r="J55">
+        <v>50</v>
+      </c>
+      <c r="K55" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>41</v>
+      </c>
+      <c r="B56" t="s">
+        <v>24</v>
+      </c>
+      <c r="C56" t="s">
+        <v>154</v>
+      </c>
+      <c r="D56" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" t="s">
+        <v>8</v>
+      </c>
+      <c r="F56" t="s">
+        <v>9</v>
+      </c>
+      <c r="G56" t="s">
+        <v>12</v>
+      </c>
+      <c r="H56" t="s">
+        <v>22</v>
+      </c>
+      <c r="I56" t="s">
+        <v>44</v>
+      </c>
+      <c r="J56">
+        <v>50</v>
+      </c>
+      <c r="K56" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated clip_loo_subjects to use dataloaders instead of loading in all data at once
</commit_message>
<xml_diff>
--- a/CLIP Model Results.xlsx
+++ b/CLIP Model Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Portable\Documents\GitHub\CMPUT624_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706C5865-90DC-4887-8FDF-B10A7F097047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED4F9A75-FF40-458B-A7D6-AC0071CE2E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="158">
   <si>
     <t>Text Input</t>
   </si>
@@ -490,6 +490,15 @@
   </si>
   <si>
     <t>(fmri channel for each word) (detrended) gaussian weighted 3D fMRI image 2-8 seconds after each word</t>
+  </si>
+  <si>
+    <t>slurm-42599447</t>
+  </si>
+  <si>
+    <t>slurm-42599773</t>
+  </si>
+  <si>
+    <t>slurm-42599776</t>
   </si>
 </sst>
 </file>
@@ -819,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q56"/>
+  <dimension ref="A1:Q57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E45" workbookViewId="0">
-      <selection activeCell="P56" sqref="P56"/>
+    <sheetView tabSelected="1" topLeftCell="E36" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3505,6 +3514,9 @@
       <c r="K55" t="s">
         <v>45</v>
       </c>
+      <c r="P55" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
@@ -3539,6 +3551,47 @@
       </c>
       <c r="K56" t="s">
         <v>45</v>
+      </c>
+      <c r="P56" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>41</v>
+      </c>
+      <c r="B57" t="s">
+        <v>28</v>
+      </c>
+      <c r="C57" t="s">
+        <v>154</v>
+      </c>
+      <c r="D57" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" t="s">
+        <v>8</v>
+      </c>
+      <c r="F57" t="s">
+        <v>9</v>
+      </c>
+      <c r="G57" t="s">
+        <v>12</v>
+      </c>
+      <c r="H57" t="s">
+        <v>22</v>
+      </c>
+      <c r="I57" t="s">
+        <v>44</v>
+      </c>
+      <c r="J57">
+        <v>50</v>
+      </c>
+      <c r="K57" t="s">
+        <v>45</v>
+      </c>
+      <c r="P57" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reverted back to summing word fmris to get results
</commit_message>
<xml_diff>
--- a/CLIP Model Results.xlsx
+++ b/CLIP Model Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Portable\Documents\GitHub\CMPUT624_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37830B8-27ED-4029-9BAA-2F74ECAC19A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86964EF6-AE1A-4A28-A72E-17699967E7AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="0" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="194">
   <si>
     <t>Text Input</t>
   </si>
@@ -597,13 +597,16 @@
     <t>slurm-42631297</t>
   </si>
   <si>
-    <t>slurm-42631336</t>
-  </si>
-  <si>
-    <t>slurm-42631341</t>
-  </si>
-  <si>
-    <t>slurm-42631351</t>
+    <t>slurm-42642165</t>
+  </si>
+  <si>
+    <t>slurm-42642207</t>
+  </si>
+  <si>
+    <t>slurm-42642224</t>
+  </si>
+  <si>
+    <t>note: these assements had the text split by the number of words so there was no overlap, thus somewhat inflating results</t>
   </si>
 </sst>
 </file>
@@ -933,10 +936,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q71"/>
+  <dimension ref="A1:Q72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F40" workbookViewId="0">
-      <selection activeCell="P70" sqref="P70"/>
+    <sheetView tabSelected="1" topLeftCell="E43" workbookViewId="0">
+      <selection activeCell="P72" sqref="P72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3704,6 +3707,9 @@
       <c r="P57" t="s">
         <v>155</v>
       </c>
+      <c r="Q57" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
@@ -3754,6 +3760,9 @@
       <c r="P58" t="s">
         <v>158</v>
       </c>
+      <c r="Q58" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
@@ -3804,6 +3813,9 @@
       <c r="P59" t="s">
         <v>156</v>
       </c>
+      <c r="Q59" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
@@ -3854,6 +3866,9 @@
       <c r="P60" t="s">
         <v>157</v>
       </c>
+      <c r="Q60" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
@@ -3892,6 +3907,9 @@
       <c r="P61" t="s">
         <v>158</v>
       </c>
+      <c r="Q61" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
@@ -3930,6 +3948,9 @@
       <c r="P62" t="s">
         <v>158</v>
       </c>
+      <c r="Q62" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
@@ -4298,6 +4319,44 @@
       </c>
       <c r="P71" t="s">
         <v>192</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>72</v>
+      </c>
+      <c r="B72" t="s">
+        <v>6</v>
+      </c>
+      <c r="C72" t="s">
+        <v>154</v>
+      </c>
+      <c r="D72" t="s">
+        <v>8</v>
+      </c>
+      <c r="E72" t="s">
+        <v>8</v>
+      </c>
+      <c r="F72" t="s">
+        <v>9</v>
+      </c>
+      <c r="G72" t="s">
+        <v>12</v>
+      </c>
+      <c r="H72" t="s">
+        <v>22</v>
+      </c>
+      <c r="I72" t="s">
+        <v>44</v>
+      </c>
+      <c r="J72">
+        <v>50</v>
+      </c>
+      <c r="K72" t="s">
+        <v>45</v>
+      </c>
+      <c r="P72" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>